<commit_message>
down load route added
</commit_message>
<xml_diff>
--- a/server/output.xlsx
+++ b/server/output.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -457,9 +457,20 @@
         <v>2025-07-03T19:48:08.209Z</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>192.168.1.28</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/138.0.0.0 Safari/537.36 Edg/138.0.0.0</v>
+      </c>
+      <c r="C6" t="str">
+        <v>2025-07-03T19:58:21.882Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>